<commit_message>
added try catch to identify which row an illegal character is in the excel
</commit_message>
<xml_diff>
--- a/Email-Automation-Bot/Demo-set.xlsx
+++ b/Email-Automation-Bot/Demo-set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Softeng762\Email-Automation-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003B5A42-A428-44F6-B55E-2482EE49DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C12349-794C-4E16-88A0-ECF39F20C75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="27555" windowHeight="11385" xr2:uid="{35F2FEA0-FCB0-43AF-A617-1082C65B0A32}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Project Category</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Human Computer Interactions 2</t>
-  </si>
-  <si>
-    <t>Garmin</t>
   </si>
   <si>
     <t>Games &amp; Education Aids 1</t>
@@ -223,91 +220,28 @@
     <t>858-2106-50</t>
   </si>
   <si>
-    <t>447-0417-33</t>
-  </si>
-  <si>
-    <t>775-3082-17</t>
-  </si>
-  <si>
-    <t>474-7865-59</t>
-  </si>
-  <si>
-    <t>907-2775-73</t>
-  </si>
-  <si>
-    <t>242-9870-85</t>
-  </si>
-  <si>
-    <t>761-2311-20</t>
-  </si>
-  <si>
-    <t>351-0106-65</t>
-  </si>
-  <si>
     <t>234-4277-82</t>
-  </si>
-  <si>
-    <t>855-4882-86</t>
-  </si>
-  <si>
-    <t>974-9797-51</t>
-  </si>
-  <si>
-    <t>163-7749-22</t>
   </si>
   <si>
     <t>893-2365-76</t>
   </si>
   <si>
-    <t>113-7707-43</t>
-  </si>
-  <si>
     <t>Roland Casey</t>
-  </si>
-  <si>
-    <t>Maria Farrell</t>
-  </si>
-  <si>
-    <t>Arnold Martin</t>
-  </si>
-  <si>
-    <t>Mike Kelly</t>
-  </si>
-  <si>
-    <t>Kellan Barrett</t>
-  </si>
-  <si>
-    <t>Byron Hawkins</t>
-  </si>
-  <si>
-    <t>Amber Alexander</t>
-  </si>
-  <si>
-    <t>Annabella Brooks</t>
   </si>
   <si>
     <t>Carl Clark</t>
   </si>
   <si>
-    <t>Alan Riley</t>
-  </si>
-  <si>
-    <t>Sam Moore</t>
-  </si>
-  <si>
-    <t>Eleanor Montgomery</t>
-  </si>
-  <si>
     <t>Luke Jones</t>
-  </si>
-  <si>
-    <t>Justin Turner</t>
   </si>
   <si>
     <t>Parrot</t>
   </si>
   <si>
-    <t>anonymous07102022@gmail.com</t>
+    <t>michellelu.lu7@gmail.com</t>
+  </si>
+  <si>
+    <t>Garmin?</t>
   </si>
 </sst>
 </file>
@@ -860,7 +794,7 @@
   <dimension ref="A1:AB996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,31 +830,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="20"/>
       <c r="L1" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
       <c r="O1" s="20"/>
       <c r="P1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="16" t="s">
         <v>60</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -992,37 +926,37 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="7" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
@@ -1048,34 +982,22 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="7"/>
       <c r="O4" s="9"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="10"/>
@@ -1100,27 +1022,21 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="M5" s="13"/>
       <c r="N5" s="7"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
@@ -1142,31 +1058,25 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="7"/>
       <c r="O6" s="9"/>
       <c r="P6" s="12"/>
@@ -1185,21 +1095,15 @@
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1225,21 +1129,15 @@
     </row>
     <row r="8" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -1265,21 +1163,15 @@
     </row>
     <row r="9" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>68</v>
-      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1305,21 +1197,15 @@
     </row>
     <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1345,10 +1231,10 @@
     </row>
     <row r="11" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="7"/>
@@ -1379,10 +1265,10 @@
     </row>
     <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="7"/>
@@ -1413,10 +1299,10 @@
     </row>
     <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="7"/>
@@ -1447,10 +1333,10 @@
     </row>
     <row r="14" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="7"/>
@@ -1481,10 +1367,10 @@
     </row>
     <row r="15" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="7"/>
@@ -1515,10 +1401,10 @@
     </row>
     <row r="16" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="7"/>
@@ -1549,10 +1435,10 @@
     </row>
     <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="7"/>
@@ -1583,10 +1469,10 @@
     </row>
     <row r="18" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="7"/>
@@ -1617,10 +1503,10 @@
     </row>
     <row r="19" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="7"/>
@@ -1651,10 +1537,10 @@
     </row>
     <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="7"/>
@@ -1685,10 +1571,10 @@
     </row>
     <row r="21" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="7"/>
@@ -1719,10 +1605,10 @@
     </row>
     <row r="22" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="7"/>
@@ -1753,10 +1639,10 @@
     </row>
     <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="7"/>
@@ -1787,10 +1673,10 @@
     </row>
     <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="7"/>
@@ -1821,10 +1707,10 @@
     </row>
     <row r="25" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="7"/>
@@ -1855,10 +1741,10 @@
     </row>
     <row r="26" spans="1:28" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="7"/>
@@ -1889,10 +1775,10 @@
     </row>
     <row r="27" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="7"/>
@@ -31006,11 +30892,11 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{56C605B3-0CFB-42D7-90AF-012367B6B480}"/>
-    <hyperlink ref="E4:E10" r:id="rId2" display="anonymous07102022@gmail.com" xr:uid="{B5D13755-AC5A-4266-9987-005B16111052}"/>
-    <hyperlink ref="I3" r:id="rId3" xr:uid="{9A05452B-A302-431E-9AC5-1816290FB218}"/>
-    <hyperlink ref="I4:I6" r:id="rId4" display="anonymous07102022@gmail.com" xr:uid="{F3807226-EF5D-41E8-AE17-5B77BB949212}"/>
-    <hyperlink ref="M3" r:id="rId5" xr:uid="{36FE0109-5E7E-4623-A3C0-366CBCE7E2E5}"/>
-    <hyperlink ref="M4" r:id="rId6" xr:uid="{099DA5CB-4B63-4B5A-BBC8-5A986F25B684}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{59ADCDEF-A5B4-4628-907B-E6EC47F521ED}"/>
+    <hyperlink ref="M3" r:id="rId3" xr:uid="{CA113A77-907E-4597-8E19-CA90103F5121}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{632D4EDA-2546-42F7-9045-C4F3B941323E}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{0E52BA5A-C3C1-4DA3-B691-162A42A6C9E4}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{54EFCA8D-ED58-4407-AF18-9274DA65E70F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>